<commit_message>
Minor fixes to the Formulario file
</commit_message>
<xml_diff>
--- a/Formulario.xlsx
+++ b/Formulario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\MÀSTER\3 - Pràcriques en empresa\Archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C5D34-6AFB-4071-801F-40DA14A1747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33510BD8-DA04-487B-B83E-5685C9861C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{0FD50DD6-E2B4-4886-A476-20BE2B7416D5}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{0FD50DD6-E2B4-4886-A476-20BE2B7416D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Quantative traits</t>
   </si>
@@ -293,7 +293,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +326,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -696,7 +704,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -716,7 +724,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -742,6 +749,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1408,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6788A869-FE23-49B8-BC49-F093554D703C}">
   <dimension ref="B2:G56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,23 +1442,23 @@
       <c r="D3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -1457,10 +1466,10 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
@@ -1468,10 +1477,10 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
@@ -1479,10 +1488,10 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
@@ -1490,10 +1499,10 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
@@ -1841,10 +1850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFDF4F7-EB60-466D-B2DD-2F25491506B0}">
-  <dimension ref="A2:E54"/>
+  <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,684 +1865,738 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="17" t="str">
+      <c r="A3" t="str">
+        <f>IF(Form!B4=0,"",Form!B4)</f>
+        <v>Plant_height</v>
+      </c>
+      <c r="B3" s="16" t="str">
         <f>IF(Form!C4=0,"",Form!C4)</f>
         <v/>
       </c>
-      <c r="C3" s="15" t="str">
+      <c r="C3" s="14" t="str">
         <f>IF(Form!D4=0,"",Form!D4)</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="14" t="str">
+      <c r="A4" t="str">
+        <f>IF(Form!B5=0,"",Form!B5)</f>
+        <v>Stem_length</v>
+      </c>
+      <c r="B4" s="13" t="str">
         <f>IF(Form!C5=0,"",Form!C5)</f>
         <v/>
       </c>
-      <c r="C4" s="16" t="str">
+      <c r="C4" s="15" t="str">
         <f>IF(Form!D5=0,"",Form!D5)</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="14" t="str">
+      <c r="A5" t="str">
+        <f>IF(Form!B6=0,"",Form!B6)</f>
+        <v>Stem_width</v>
+      </c>
+      <c r="B5" s="13" t="str">
         <f>IF(Form!C6=0,"",Form!C6)</f>
         <v/>
       </c>
-      <c r="C5" s="16" t="str">
+      <c r="C5" s="15" t="str">
         <f>IF(Form!D6=0,"",Form!D6)</f>
         <v/>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="14" t="str">
+      <c r="A6" t="str">
+        <f>IF(Form!B7=0,"",Form!B7)</f>
+        <v>Leaf_sheat_length</v>
+      </c>
+      <c r="B6" s="13" t="str">
         <f>IF(Form!C7=0,"",Form!C7)</f>
         <v/>
       </c>
-      <c r="C6" s="16" t="str">
+      <c r="C6" s="15" t="str">
         <f>IF(Form!D7=0,"",Form!D7)</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="14" t="str">
+      <c r="A7" t="str">
+        <f>IF(Form!B8=0,"",Form!B8)</f>
+        <v>Petiole_length</v>
+      </c>
+      <c r="B7" s="13" t="str">
         <f>IF(Form!C8=0,"",Form!C8)</f>
         <v/>
       </c>
-      <c r="C7" s="16" t="str">
+      <c r="C7" s="15" t="str">
         <f>IF(Form!D8=0,"",Form!D8)</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="14" t="str">
+      <c r="A8" t="str">
+        <f>IF(Form!B9=0,"",Form!B9)</f>
+        <v>Petiole_thickness</v>
+      </c>
+      <c r="B8" s="13" t="str">
         <f>IF(Form!C9=0,"",Form!C9)</f>
         <v/>
       </c>
-      <c r="C8" s="16" t="str">
+      <c r="C8" s="15" t="str">
         <f>IF(Form!D9=0,"",Form!D9)</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="14" t="str">
+      <c r="A9" t="str">
+        <f>IF(Form!B10=0,"",Form!B10)</f>
+        <v>Peduncle_length</v>
+      </c>
+      <c r="B9" s="13" t="str">
         <f>IF(Form!C10=0,"",Form!C10)</f>
         <v/>
       </c>
-      <c r="C9" s="16" t="str">
+      <c r="C9" s="15" t="str">
         <f>IF(Form!D10=0,"",Form!D10)</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="14" t="str">
+      <c r="A10" t="str">
+        <f>IF(Form!B11=0,"",Form!B11)</f>
+        <v>Peduncle_width</v>
+      </c>
+      <c r="B10" s="13" t="str">
         <f>IF(Form!C11=0,"",Form!C11)</f>
         <v/>
       </c>
-      <c r="C10" s="16" t="str">
+      <c r="C10" s="15" t="str">
         <f>IF(Form!D11=0,"",Form!D11)</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="14" t="str">
+      <c r="A11" t="str">
+        <f>IF(Form!B12=0,"",Form!B12)</f>
+        <v>Distance_scar_bracteole</v>
+      </c>
+      <c r="B11" s="13" t="str">
         <f>IF(Form!C12=0,"",Form!C12)</f>
         <v/>
       </c>
-      <c r="C11" s="16" t="str">
+      <c r="C11" s="15" t="str">
         <f>IF(Form!D12=0,"",Form!D12)</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="14" t="str">
+      <c r="A12" t="str">
+        <f>IF(Form!B13=0,"",Form!B13)</f>
+        <v>Prophyll_length</v>
+      </c>
+      <c r="B12" s="13" t="str">
         <f>IF(Form!C13=0,"",Form!C13)</f>
         <v/>
       </c>
-      <c r="C12" s="16" t="str">
+      <c r="C12" s="15" t="str">
         <f>IF(Form!D13=0,"",Form!D13)</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="14" t="str">
+      <c r="A13" t="str">
+        <f>IF(Form!B14=0,"",Form!B14)</f>
+        <v>Peduncle_bract_length</v>
+      </c>
+      <c r="B13" s="13" t="str">
         <f>IF(Form!C14=0,"",Form!C14)</f>
         <v/>
       </c>
-      <c r="C13" s="16" t="str">
+      <c r="C13" s="15" t="str">
         <f>IF(Form!D14=0,"",Form!D14)</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="14" t="str">
+      <c r="A14" t="str">
+        <f>IF(Form!B15=0,"",Form!B15)</f>
+        <v>Apical_leaflet_length</v>
+      </c>
+      <c r="B14" s="13" t="str">
         <f>IF(Form!C15=0,"",Form!C15)</f>
         <v/>
       </c>
-      <c r="C14" s="16" t="str">
+      <c r="C14" s="15" t="str">
         <f>IF(Form!D15=0,"",Form!D15)</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="14" t="str">
+      <c r="A15" t="str">
+        <f>IF(Form!B16=0,"",Form!B16)</f>
+        <v>Apical_leaflet_width</v>
+      </c>
+      <c r="B15" s="13" t="str">
         <f>IF(Form!C16=0,"",Form!C16)</f>
         <v/>
       </c>
-      <c r="C15" s="16" t="str">
+      <c r="C15" s="15" t="str">
         <f>IF(Form!D16=0,"",Form!D16)</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="14" t="str">
+      <c r="A16" t="str">
+        <f>IF(Form!B17=0,"",Form!B17)</f>
+        <v>Apical_leaflet_angle</v>
+      </c>
+      <c r="B16" s="13" t="str">
         <f>IF(Form!C17=0,"",Form!C17)</f>
         <v/>
       </c>
-      <c r="C16" s="16" t="str">
+      <c r="C16" s="15" t="str">
         <f>IF(Form!D17=0,"",Form!D17)</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="14" t="str">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>IF(Form!B18=0,"",Form!B18)</f>
+        <v>Apical_leaflet_vein_count</v>
+      </c>
+      <c r="B17" s="13" t="str">
         <f>IF(Form!C18=0,"",Form!C18)</f>
         <v/>
       </c>
-      <c r="C17" s="16" t="str">
+      <c r="C17" s="15" t="str">
         <f>IF(Form!D18=0,"",Form!D18)</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="14" t="str">
+      <c r="G17" s="32"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>IF(Form!B19=0,"",Form!B19)</f>
+        <v>Basal_leaflet_angle</v>
+      </c>
+      <c r="B18" s="13" t="str">
         <f>IF(Form!C19=0,"",Form!C19)</f>
         <v/>
       </c>
-      <c r="C18" s="16" t="str">
+      <c r="C18" s="15" t="str">
         <f>IF(Form!D19=0,"",Form!D19)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="14" t="str">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>IF(Form!B20=0,"",Form!B20)</f>
+        <v>Basal_leaflet_length</v>
+      </c>
+      <c r="B19" s="13" t="str">
         <f>IF(Form!C20=0,"",Form!C20)</f>
         <v/>
       </c>
-      <c r="C19" s="16" t="str">
+      <c r="C19" s="15" t="str">
         <f>IF(Form!D20=0,"",Form!D20)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="14" t="str">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>IF(Form!B21=0,"",Form!B21)</f>
+        <v>Basal_leaflet_width</v>
+      </c>
+      <c r="B20" s="13" t="str">
         <f>IF(Form!C21=0,"",Form!C21)</f>
         <v/>
       </c>
-      <c r="C20" s="16" t="str">
+      <c r="C20" s="15" t="str">
         <f>IF(Form!D21=0,"",Form!D21)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="14" t="str">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>IF(Form!B22=0,"",Form!B22)</f>
+        <v>Median_leaflet_length</v>
+      </c>
+      <c r="B21" s="13" t="str">
         <f>IF(Form!C22=0,"",Form!C22)</f>
         <v/>
       </c>
-      <c r="C21" s="16" t="str">
+      <c r="C21" s="15" t="str">
         <f>IF(Form!D22=0,"",Form!D22)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="14" t="str">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>IF(Form!B23=0,"",Form!B23)</f>
+        <v>Median_leaflet_width</v>
+      </c>
+      <c r="B22" s="13" t="str">
         <f>IF(Form!C23=0,"",Form!C23)</f>
         <v/>
       </c>
-      <c r="C22" s="16" t="str">
+      <c r="C22" s="15" t="str">
         <f>IF(Form!D23=0,"",Form!D23)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="14" t="str">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>IF(Form!B24=0,"",Form!B24)</f>
+        <v>Leaflet_number</v>
+      </c>
+      <c r="B23" s="13" t="str">
         <f>IF(Form!C24=0,"",Form!C24)</f>
         <v/>
       </c>
-      <c r="C23" s="16" t="str">
+      <c r="C23" s="15" t="str">
         <f>IF(Form!D24=0,"",Form!D24)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="14" t="str">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>IF(Form!B25=0,"",Form!B25)</f>
+        <v>Rachis_length</v>
+      </c>
+      <c r="B24" s="13" t="str">
         <f>IF(Form!C25=0,"",Form!C25)</f>
         <v/>
       </c>
-      <c r="C24" s="16" t="str">
+      <c r="C24" s="15" t="str">
         <f>IF(Form!D25=0,"",Form!D25)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="14" t="str">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>IF(Form!B26=0,"",Form!B26)</f>
+        <v>Rachis_thickness</v>
+      </c>
+      <c r="B25" s="13" t="str">
         <f>IF(Form!C26=0,"",Form!C26)</f>
         <v/>
       </c>
-      <c r="C25" s="16" t="str">
+      <c r="C25" s="15" t="str">
         <f>IF(Form!D26=0,"",Form!D26)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="14" t="str">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>IF(Form!B27=0,"",Form!B27)</f>
+        <v>Rachilla_count</v>
+      </c>
+      <c r="B26" s="13" t="str">
         <f>IF(Form!C27=0,"",Form!C27)</f>
         <v/>
       </c>
-      <c r="C26" s="16" t="str">
+      <c r="C26" s="15" t="str">
         <f>IF(Form!D27=0,"",Form!D27)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="14" t="str">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>IF(Form!B28=0,"",Form!B28)</f>
+        <v>Rachilla_length</v>
+      </c>
+      <c r="B27" s="13" t="str">
         <f>IF(Form!C28=0,"",Form!C28)</f>
         <v/>
       </c>
-      <c r="C27" s="16" t="str">
+      <c r="C27" s="15" t="str">
         <f>IF(Form!D28=0,"",Form!D28)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="14" t="str">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>IF(Form!B29=0,"",Form!B29)</f>
+        <v>Rachilla_thickness</v>
+      </c>
+      <c r="B28" s="13" t="str">
         <f>IF(Form!C29=0,"",Form!C29)</f>
         <v/>
       </c>
-      <c r="C28" s="16" t="str">
+      <c r="C28" s="15" t="str">
         <f>IF(Form!D29=0,"",Form!D29)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="14" t="str">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>IF(Form!B30=0,"",Form!B30)</f>
+        <v>Staminate_rachilla_length</v>
+      </c>
+      <c r="B29" s="13" t="str">
         <f>IF(Form!C30=0,"",Form!C30)</f>
         <v/>
       </c>
-      <c r="C29" s="16" t="str">
+      <c r="C29" s="15" t="str">
         <f>IF(Form!D30=0,"",Form!D30)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="14" t="str">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>IF(Form!B31=0,"",Form!B31)</f>
+        <v>Staminate_rachilla_count</v>
+      </c>
+      <c r="B30" s="13" t="str">
         <f>IF(Form!C31=0,"",Form!C31)</f>
         <v/>
       </c>
-      <c r="C30" s="16" t="str">
+      <c r="C30" s="15" t="str">
         <f>IF(Form!D31=0,"",Form!D31)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="14" t="str">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>IF(Form!B32=0,"",Form!B32)</f>
+        <v>Pistillate_rachilla_length</v>
+      </c>
+      <c r="B31" s="13" t="str">
         <f>IF(Form!C32=0,"",Form!C32)</f>
         <v/>
       </c>
-      <c r="C31" s="16" t="str">
+      <c r="C31" s="15" t="str">
         <f>IF(Form!D32=0,"",Form!D32)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="14" t="str">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>IF(Form!B33=0,"",Form!B33)</f>
+        <v>Pistillate_rachilla_count</v>
+      </c>
+      <c r="B32" s="13" t="str">
         <f>IF(Form!C33=0,"",Form!C33)</f>
         <v/>
       </c>
-      <c r="C32" s="16" t="str">
+      <c r="C32" s="15" t="str">
         <f>IF(Form!D33=0,"",Form!D33)</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="14" t="str">
+      <c r="A33" t="str">
+        <f>IF(Form!B34=0,"",Form!B34)</f>
+        <v>Basal_rachilla_length</v>
+      </c>
+      <c r="B33" s="13" t="str">
         <f>IF(Form!C34=0,"",Form!C34)</f>
         <v/>
       </c>
-      <c r="C33" s="16" t="str">
+      <c r="C33" s="15" t="str">
         <f>IF(Form!D34=0,"",Form!D34)</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="14" t="str">
+      <c r="A34" t="str">
+        <f>IF(Form!B35=0,"",Form!B35)</f>
+        <v>Basal_rachilla_thickness</v>
+      </c>
+      <c r="B34" s="13" t="str">
         <f>IF(Form!C35=0,"",Form!C35)</f>
         <v/>
       </c>
-      <c r="C34" s="16" t="str">
+      <c r="C34" s="15" t="str">
         <f>IF(Form!D35=0,"",Form!D35)</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="14" t="str">
+      <c r="A35" t="str">
+        <f>IF(Form!B36=0,"",Form!B36)</f>
+        <v>Apical_rachilla_length</v>
+      </c>
+      <c r="B35" s="13" t="str">
         <f>IF(Form!C36=0,"",Form!C36)</f>
         <v/>
       </c>
-      <c r="C35" s="16" t="str">
+      <c r="C35" s="15" t="str">
         <f>IF(Form!D36=0,"",Form!D36)</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="14" t="str">
+      <c r="A36" t="str">
+        <f>IF(Form!B37=0,"",Form!B37)</f>
+        <v>Apical_rachilla_thickness</v>
+      </c>
+      <c r="B36" s="13" t="str">
         <f>IF(Form!C37=0,"",Form!C37)</f>
         <v/>
       </c>
-      <c r="C36" s="16" t="str">
+      <c r="C36" s="15" t="str">
         <f>IF(Form!D37=0,"",Form!D37)</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="14" t="str">
+      <c r="A37" t="str">
+        <f>IF(Form!B38=0,"",Form!B38)</f>
+        <v>Median_rachilla_length</v>
+      </c>
+      <c r="B37" s="13" t="str">
         <f>IF(Form!C38=0,"",Form!C38)</f>
         <v/>
       </c>
-      <c r="C37" s="16" t="str">
+      <c r="C37" s="15" t="str">
         <f>IF(Form!D38=0,"",Form!D38)</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="14" t="str">
+      <c r="A38" t="str">
+        <f>IF(Form!B39=0,"",Form!B39)</f>
+        <v>Fruit_length</v>
+      </c>
+      <c r="B38" s="13" t="str">
         <f>IF(Form!C39=0,"",Form!C39)</f>
         <v/>
       </c>
-      <c r="C38" s="16" t="str">
+      <c r="C38" s="15" t="str">
         <f>IF(Form!D39=0,"",Form!D39)</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="14" t="str">
+      <c r="A39" t="str">
+        <f>IF(Form!B40=0,"",Form!B40)</f>
+        <v>Fruit_width</v>
+      </c>
+      <c r="B39" s="13" t="str">
         <f>IF(Form!C40=0,"",Form!C40)</f>
         <v/>
       </c>
-      <c r="C39" s="16" t="str">
+      <c r="C39" s="15" t="str">
         <f>IF(Form!D40=0,"",Form!D40)</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="14" t="str">
+      <c r="A40" t="str">
+        <f>IF(Form!B41=0,"",Form!B41)</f>
+        <v>Seed_length</v>
+      </c>
+      <c r="B40" s="13" t="str">
         <f>IF(Form!C41=0,"",Form!C41)</f>
         <v/>
       </c>
-      <c r="C40" s="16" t="str">
+      <c r="C40" s="15" t="str">
         <f>IF(Form!D41=0,"",Form!D41)</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="14" t="str">
+      <c r="A41" t="str">
+        <f>IF(Form!B42=0,"",Form!B42)</f>
+        <v>Seed_width</v>
+      </c>
+      <c r="B41" s="13" t="str">
         <f>IF(Form!C42=0,"",Form!C42)</f>
         <v/>
       </c>
-      <c r="C41" s="16" t="str">
+      <c r="C41" s="15" t="str">
         <f>IF(Form!D42=0,"",Form!D42)</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="14" t="str">
+      <c r="A42" t="str">
+        <f>IF(Form!B43=0,"",Form!B43)</f>
+        <v>Seed_count</v>
+      </c>
+      <c r="B42" s="13" t="str">
         <f>IF(Form!C43=0,"",Form!C43)</f>
         <v/>
       </c>
-      <c r="C42" s="16" t="str">
+      <c r="C42" s="15" t="str">
         <f>IF(Form!D43=0,"",Form!D43)</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="14" t="str">
+      <c r="A43" t="str">
+        <f>IF(Form!B44=0,"",Form!B44)</f>
+        <v>Stamen_count</v>
+      </c>
+      <c r="B43" s="13" t="str">
         <f>IF(Form!C44=0,"",Form!C44)</f>
         <v/>
       </c>
-      <c r="C43" s="16" t="str">
+      <c r="C43" s="15" t="str">
         <f>IF(Form!D44=0,"",Form!D44)</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="14" t="str">
+      <c r="A44" t="str">
+        <f>IF(Form!B45=0,"",Form!B45)</f>
+        <v>Inflorescence_branch_count</v>
+      </c>
+      <c r="B44" s="13" t="str">
         <f>IF(Form!C45=0,"",Form!C45)</f>
         <v/>
       </c>
-      <c r="C44" s="16" t="str">
+      <c r="C44" s="15" t="str">
         <f>IF(Form!D45=0,"",Form!D45)</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="14" t="str">
+      <c r="A45" t="str">
+        <f>IF(Form!B46=0,"",Form!B46)</f>
+        <v>Inflorescence_length</v>
+      </c>
+      <c r="B45" s="13" t="str">
         <f>IF(Form!C46=0,"",Form!C46)</f>
         <v/>
       </c>
-      <c r="C45" s="16" t="str">
+      <c r="C45" s="15" t="str">
         <f>IF(Form!D46=0,"",Form!D46)</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="14" t="str">
+      <c r="A46" t="str">
+        <f>IF(Form!B47=0,"",Form!B47)</f>
+        <v>Inflorescence_width</v>
+      </c>
+      <c r="B46" s="13" t="str">
         <f>IF(Form!C47=0,"",Form!C47)</f>
         <v/>
       </c>
-      <c r="C46" s="16" t="str">
+      <c r="C46" s="15" t="str">
         <f>IF(Form!D47=0,"",Form!D47)</f>
         <v/>
       </c>
-      <c r="E46" s="31"/>
+      <c r="E46" s="30"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="14" t="str">
+      <c r="A47" t="str">
+        <f>IF(Form!B48=0,"",Form!B48)</f>
+        <v>Staminate_inflorescence_length</v>
+      </c>
+      <c r="B47" s="13" t="str">
         <f>IF(Form!C48=0,"",Form!C48)</f>
         <v/>
       </c>
-      <c r="C47" s="16" t="str">
+      <c r="C47" s="15" t="str">
         <f>IF(Form!D48=0,"",Form!D48)</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="14" t="str">
+      <c r="A48" t="str">
+        <f>IF(Form!B49=0,"",Form!B49)</f>
+        <v>Pistillate_inflorescence_length</v>
+      </c>
+      <c r="B48" s="13" t="str">
         <f>IF(Form!C49=0,"",Form!C49)</f>
         <v/>
       </c>
-      <c r="C48" s="16" t="str">
+      <c r="C48" s="15" t="str">
         <f>IF(Form!D49=0,"",Form!D49)</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="14" t="str">
+      <c r="A49" t="str">
+        <f>IF(Form!B50=0,"",Form!B50)</f>
+        <v>Staminate_flower_length</v>
+      </c>
+      <c r="B49" s="13" t="str">
         <f>IF(Form!C50=0,"",Form!C50)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C49" s="16" t="str">
+      <c r="C49" s="15" t="str">
         <f>IF(Form!D50=0,"",Form!D50)</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="14" t="str">
+      <c r="A50" t="str">
+        <f>IF(Form!B51=0,"",Form!B51)</f>
+        <v>Shoot_axis_internode_length</v>
+      </c>
+      <c r="B50" s="13" t="str">
         <f>IF(Form!C51=0,"",Form!C51)</f>
         <v/>
       </c>
-      <c r="C50" s="16" t="str">
+      <c r="C50" s="15" t="str">
         <f>IF(Form!D51=0,"",Form!D51)</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="14" t="str">
+      <c r="A51" t="str">
+        <f>IF(Form!B52=0,"",Form!B52)</f>
+        <v>Leaf_number</v>
+      </c>
+      <c r="B51" s="13" t="str">
         <f>IF(Form!C52=0,"",Form!C52)</f>
         <v/>
       </c>
-      <c r="C51" s="16" t="str">
+      <c r="C51" s="15" t="str">
         <f>IF(Form!D52=0,"",Form!D52)</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="14" t="str">
+      <c r="A52" t="str">
+        <f>IF(Form!B53=0,"",Form!B53)</f>
+        <v>Bracts_number</v>
+      </c>
+      <c r="B52" s="13" t="str">
         <f>IF(Form!C53=0,"",Form!C53)</f>
         <v/>
       </c>
-      <c r="C52" s="20" t="str">
+      <c r="C52" s="19" t="str">
         <f>IF([1]Form!G47=0,"",[1]Form!G47)</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="19" t="str">
+      <c r="A53" t="str">
+        <f>IF(Form!F4=0,"",Form!F4)</f>
+        <v>measurementDeterminedDate</v>
+      </c>
+      <c r="B53" s="18" t="str">
         <f>IF(Form!G4=0,"",Form!G4)</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="21" t="str">
+      <c r="A54" t="str">
+        <f>IF(Form!F5=0,"",Form!F5)</f>
+        <v>measurementDeterminedBy</v>
+      </c>
+      <c r="B54" s="20" t="str">
         <f>IF(Form!G5=0,"",Form!G5)</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>